<commit_message>
Removed options for null entries
</commit_message>
<xml_diff>
--- a/xlsx/form_b_lideres.xlsx
+++ b/xlsx/form_b_lideres.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23426"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Terra_Share\projects\CaVaTeCo_Collect\projects\odk_forms_cesc_niassa\xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Terra_Share\projects\CaVaTeCo_Collect\projects\monitor_forms\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F61E71A3-FDA2-4E2D-A59C-C4CF50F72547}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E53DDD5-FDEC-4A23-8814-AD0050CEDA73}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1114" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1112" uniqueCount="219">
   <si>
     <t>type</t>
   </si>
@@ -666,9 +666,6 @@
     <t>village_name</t>
   </si>
   <si>
-    <t>Outro povoado (não está na lista)</t>
-  </si>
-  <si>
     <t>languages</t>
   </si>
   <si>
@@ -681,6 +678,9 @@
     <t>concat('Village','_',${village_id})</t>
   </si>
   <si>
+    <t>"CESC Niassa"</t>
+  </si>
+  <si>
     <t>search('enum_names_cesc_niassa')</t>
   </si>
   <si>
@@ -688,9 +688,6 @@
   </si>
   <si>
     <t>http://cavateco.terrafirma.co.mz:8080/cesc_niassa/submission</t>
-  </si>
-  <si>
-    <t>"CESC Niassa"</t>
   </si>
 </sst>
 </file>
@@ -1253,7 +1250,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1392,9 +1389,6 @@
     </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1996,7 +1990,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S52"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="I2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -2122,8 +2116,8 @@
       <c r="B6" s="52" t="s">
         <v>158</v>
       </c>
-      <c r="N6" s="69" t="s">
-        <v>219</v>
+      <c r="N6" s="68" t="s">
+        <v>215</v>
       </c>
     </row>
     <row r="7" spans="1:19" s="26" customFormat="1" x14ac:dyDescent="0.25">
@@ -2185,7 +2179,7 @@
       <c r="B12" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="C12" s="68" t="s">
+      <c r="C12" s="67" t="s">
         <v>164</v>
       </c>
     </row>
@@ -2727,10 +2721,10 @@
         <v>21</v>
       </c>
       <c r="B42" s="22" t="s">
+        <v>212</v>
+      </c>
+      <c r="C42" s="2" t="s">
         <v>213</v>
-      </c>
-      <c r="C42" s="2" t="s">
-        <v>214</v>
       </c>
     </row>
     <row r="43" spans="1:19" s="19" customFormat="1" x14ac:dyDescent="0.25">
@@ -2895,13 +2889,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C28" sqref="C28"/>
+      <selection pane="bottomRight" activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3078,17 +3072,6 @@
       </c>
       <c r="C18" s="64" t="s">
         <v>210</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="64" t="s">
-        <v>208</v>
-      </c>
-      <c r="B19" s="66">
-        <v>1</v>
-      </c>
-      <c r="C19" s="64" t="s">
-        <v>211</v>
       </c>
     </row>
   </sheetData>
@@ -7880,22 +7863,22 @@
     </row>
     <row r="845" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A845" s="44" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="846" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A846" s="44" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="847" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A847" s="44" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="848" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A848" s="44" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
   </sheetData>
@@ -7909,7 +7892,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:D2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7947,13 +7930,13 @@
         <v>161</v>
       </c>
       <c r="C2" s="30">
-        <v>202009211</v>
+        <v>202101081</v>
       </c>
       <c r="D2" s="50" t="s">
         <v>218</v>
       </c>
-      <c r="E2" s="67" t="s">
-        <v>215</v>
+      <c r="E2" s="66" t="s">
+        <v>214</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">

</xml_diff>